<commit_message>
No54 update invoice format
</commit_message>
<xml_diff>
--- a/src/HanbaiKanri/HanbaiKanri/bin/BaseXls/CollectiveInvoice.xlsx
+++ b/src/HanbaiKanri/HanbaiKanri/bin/BaseXls/CollectiveInvoice.xlsx
@@ -38,10 +38,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>MAKER</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>QUANTITY</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -174,6 +170,9 @@
   </si>
   <si>
     <t>PO No.</t>
+  </si>
+  <si>
+    <t>ITEM DESCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -457,7 +456,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -518,12 +517,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -638,6 +631,30 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -653,71 +670,47 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1091,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A18"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="12.75"/>
@@ -1112,15 +1105,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75">
-      <c r="A1" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
+      <c r="A1" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1145,15 +1138,15 @@
       <c r="AC1" s="2"/>
     </row>
     <row r="2" spans="1:29">
-      <c r="A2" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
+      <c r="A2" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1178,15 +1171,15 @@
       <c r="AC2" s="2"/>
     </row>
     <row r="3" spans="1:29">
-      <c r="A3" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
+      <c r="A3" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1211,15 +1204,15 @@
       <c r="AC3" s="2"/>
     </row>
     <row r="4" spans="1:29" ht="15">
-      <c r="A4" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
+      <c r="A4" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1244,13 +1237,13 @@
       <c r="AC4" s="2"/>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="45"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1275,15 +1268,15 @@
       <c r="AC5" s="2"/>
     </row>
     <row r="6" spans="1:29" ht="12.75" customHeight="1">
-      <c r="A6" s="63" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
+      <c r="A6" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1308,13 +1301,13 @@
       <c r="AC6" s="2"/>
     </row>
     <row r="7" spans="1:29" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A7" s="64"/>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
+      <c r="A7" s="70"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1339,175 +1332,175 @@
       <c r="AC7" s="2"/>
     </row>
     <row r="8" spans="1:29" ht="14.1" customHeight="1" thickTop="1">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="14"/>
-      <c r="E8" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="39"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="39"/>
-      <c r="X8" s="39"/>
-      <c r="Y8" s="39"/>
-      <c r="Z8" s="39"/>
-      <c r="AA8" s="39"/>
-      <c r="AB8" s="39"/>
-      <c r="AC8" s="39"/>
+      <c r="E8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="37"/>
+      <c r="U8" s="37"/>
+      <c r="V8" s="37"/>
+      <c r="W8" s="37"/>
+      <c r="X8" s="37"/>
+      <c r="Y8" s="37"/>
+      <c r="Z8" s="37"/>
+      <c r="AA8" s="37"/>
+      <c r="AB8" s="37"/>
+      <c r="AC8" s="37"/>
     </row>
     <row r="9" spans="1:29" ht="14.1" customHeight="1">
       <c r="A9" s="15"/>
-      <c r="B9" s="73"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="40"/>
+        <v>20</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="38"/>
       <c r="G9" s="16"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="39"/>
-      <c r="U9" s="39"/>
-      <c r="V9" s="39"/>
-      <c r="W9" s="39"/>
-      <c r="X9" s="39"/>
-      <c r="Y9" s="39"/>
-      <c r="Z9" s="39"/>
-      <c r="AA9" s="39"/>
-      <c r="AB9" s="39"/>
-      <c r="AC9" s="39"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37"/>
+      <c r="X9" s="37"/>
+      <c r="Y9" s="37"/>
+      <c r="Z9" s="37"/>
+      <c r="AA9" s="37"/>
+      <c r="AB9" s="37"/>
+      <c r="AC9" s="37"/>
     </row>
     <row r="10" spans="1:29" ht="14.1" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="73"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="23"/>
-      <c r="U10" s="39"/>
-      <c r="V10" s="41"/>
-      <c r="W10" s="41"/>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
-      <c r="Z10" s="41"/>
-      <c r="AA10" s="41"/>
-      <c r="AB10" s="41"/>
-      <c r="AC10" s="41"/>
+        <v>21</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="38"/>
+      <c r="G10" s="21"/>
+      <c r="U10" s="37"/>
+      <c r="V10" s="39"/>
+      <c r="W10" s="39"/>
+      <c r="X10" s="39"/>
+      <c r="Y10" s="39"/>
+      <c r="Z10" s="39"/>
+      <c r="AA10" s="39"/>
+      <c r="AB10" s="39"/>
+      <c r="AC10" s="39"/>
     </row>
     <row r="11" spans="1:29" ht="14.1" customHeight="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="73"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="23"/>
-      <c r="U11" s="39"/>
-      <c r="V11" s="42"/>
-      <c r="W11" s="43"/>
-      <c r="X11" s="43"/>
-      <c r="Y11" s="43"/>
-      <c r="Z11" s="43"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="43"/>
-      <c r="AC11" s="43"/>
+        <v>22</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="21"/>
+      <c r="U11" s="37"/>
+      <c r="V11" s="40"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="41"/>
+      <c r="AB11" s="41"/>
+      <c r="AC11" s="41"/>
     </row>
     <row r="12" spans="1:29" ht="14.1" customHeight="1">
       <c r="A12" s="4"/>
-      <c r="B12" s="73"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="23"/>
-      <c r="U12" s="39"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="41"/>
-      <c r="AA12" s="41"/>
-      <c r="AB12" s="41"/>
-      <c r="AC12" s="41"/>
+        <v>23</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="24"/>
+      <c r="G12" s="21"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="39"/>
+      <c r="W12" s="39"/>
+      <c r="X12" s="39"/>
+      <c r="Y12" s="39"/>
+      <c r="Z12" s="39"/>
+      <c r="AA12" s="39"/>
+      <c r="AB12" s="39"/>
+      <c r="AC12" s="39"/>
     </row>
     <row r="13" spans="1:29" ht="14.1" customHeight="1">
       <c r="A13" s="3"/>
-      <c r="B13" s="44"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="66"/>
-      <c r="G13" s="67"/>
-      <c r="U13" s="39"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
-      <c r="Z13" s="41"/>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="41"/>
-      <c r="AC13" s="41"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="59"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="39"/>
+      <c r="W13" s="39"/>
+      <c r="X13" s="39"/>
+      <c r="Y13" s="39"/>
+      <c r="Z13" s="39"/>
+      <c r="AA13" s="39"/>
+      <c r="AB13" s="39"/>
+      <c r="AC13" s="39"/>
     </row>
     <row r="14" spans="1:29" ht="14.1" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="66"/>
-      <c r="G14" s="67"/>
-      <c r="U14" s="39"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="41"/>
-      <c r="Y14" s="41"/>
-      <c r="Z14" s="41"/>
-      <c r="AA14" s="41"/>
-      <c r="AB14" s="41"/>
-      <c r="AC14" s="41"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="59"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="39"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="39"/>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="39"/>
+      <c r="AB14" s="39"/>
+      <c r="AC14" s="39"/>
     </row>
     <row r="15" spans="1:29" ht="14.1" customHeight="1" thickBot="1">
       <c r="A15" s="6"/>
@@ -1515,20 +1508,20 @@
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="69"/>
-      <c r="U15" s="39"/>
-      <c r="V15" s="41"/>
-      <c r="W15" s="41"/>
-      <c r="X15" s="41"/>
-      <c r="Y15" s="41"/>
-      <c r="Z15" s="41"/>
-      <c r="AA15" s="41"/>
-      <c r="AB15" s="41"/>
-      <c r="AC15" s="41"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="61"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="39"/>
+      <c r="W15" s="39"/>
+      <c r="X15" s="39"/>
+      <c r="Y15" s="39"/>
+      <c r="Z15" s="39"/>
+      <c r="AA15" s="39"/>
+      <c r="AB15" s="39"/>
+      <c r="AC15" s="39"/>
     </row>
     <row r="16" spans="1:29" ht="13.5" thickTop="1">
-      <c r="A16" s="46"/>
+      <c r="A16" s="44"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -1553,26 +1546,26 @@
       <c r="AC16" s="9"/>
     </row>
     <row r="17" spans="1:29">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="85" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="85" t="s">
+      <c r="E17" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="70" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="32" t="s">
+      <c r="G17" s="30" t="s">
         <v>5</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>6</v>
       </c>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
@@ -1598,13 +1591,13 @@
       <c r="AC17" s="11"/>
     </row>
     <row r="18" spans="1:29">
-      <c r="A18" s="71"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
+      <c r="A18" s="63"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -1631,162 +1624,162 @@
     <row r="19" spans="1:29" ht="45.75" customHeight="1">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="45"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="49"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="47"/>
     </row>
     <row r="20" spans="1:29" ht="45.75" customHeight="1">
       <c r="A20" s="8"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="45"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="56"/>
-      <c r="R20" s="56"/>
-      <c r="S20" s="56"/>
-      <c r="T20" s="56"/>
-      <c r="U20" s="56"/>
-      <c r="V20" s="56"/>
-      <c r="W20" s="56"/>
-      <c r="X20" s="56"/>
-      <c r="Y20" s="56"/>
-      <c r="Z20" s="56"/>
-      <c r="AA20" s="56"/>
-      <c r="AB20" s="56"/>
-      <c r="AC20" s="56"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="54"/>
+      <c r="T20" s="54"/>
+      <c r="U20" s="54"/>
+      <c r="V20" s="54"/>
+      <c r="W20" s="54"/>
+      <c r="X20" s="54"/>
+      <c r="Y20" s="54"/>
+      <c r="Z20" s="54"/>
+      <c r="AA20" s="54"/>
+      <c r="AB20" s="54"/>
+      <c r="AC20" s="54"/>
     </row>
     <row r="21" spans="1:29" ht="45.75" customHeight="1">
       <c r="A21" s="8"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="43"/>
-      <c r="R21" s="54"/>
-      <c r="S21" s="54"/>
-      <c r="T21" s="54"/>
-      <c r="U21" s="54"/>
-      <c r="V21" s="54"/>
-      <c r="W21" s="54"/>
-      <c r="X21" s="54"/>
-      <c r="Y21" s="54"/>
-      <c r="Z21" s="54"/>
-      <c r="AA21" s="54"/>
-      <c r="AB21" s="54"/>
-      <c r="AC21" s="54"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="R21" s="52"/>
+      <c r="S21" s="52"/>
+      <c r="T21" s="52"/>
+      <c r="U21" s="52"/>
+      <c r="V21" s="52"/>
+      <c r="W21" s="52"/>
+      <c r="X21" s="52"/>
+      <c r="Y21" s="52"/>
+      <c r="Z21" s="52"/>
+      <c r="AA21" s="52"/>
+      <c r="AB21" s="52"/>
+      <c r="AC21" s="52"/>
     </row>
     <row r="22" spans="1:29" ht="14.1" customHeight="1">
-      <c r="A22" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="65"/>
+      <c r="A22" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="84"/>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="43"/>
-      <c r="R22" s="54"/>
-      <c r="S22" s="54"/>
-      <c r="T22" s="54"/>
-      <c r="U22" s="54"/>
-      <c r="V22" s="54"/>
-      <c r="W22" s="54"/>
-      <c r="X22" s="54"/>
-      <c r="Y22" s="54"/>
-      <c r="Z22" s="54"/>
-      <c r="AA22" s="54"/>
-      <c r="AB22" s="54"/>
-      <c r="AC22" s="54"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="R22" s="52"/>
+      <c r="S22" s="52"/>
+      <c r="T22" s="52"/>
+      <c r="U22" s="52"/>
+      <c r="V22" s="52"/>
+      <c r="W22" s="52"/>
+      <c r="X22" s="52"/>
+      <c r="Y22" s="52"/>
+      <c r="Z22" s="52"/>
+      <c r="AA22" s="52"/>
+      <c r="AB22" s="52"/>
+      <c r="AC22" s="52"/>
     </row>
     <row r="23" spans="1:29" ht="14.1" customHeight="1">
-      <c r="A23" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="65"/>
+      <c r="A23" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="84"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="R23" s="54"/>
-      <c r="S23" s="54"/>
-      <c r="T23" s="54"/>
-      <c r="U23" s="54"/>
-      <c r="V23" s="54"/>
-      <c r="W23" s="54"/>
-      <c r="X23" s="54"/>
-      <c r="Y23" s="54"/>
-      <c r="Z23" s="54"/>
-      <c r="AA23" s="54"/>
-      <c r="AB23" s="54"/>
-      <c r="AC23" s="54"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="R23" s="52"/>
+      <c r="S23" s="52"/>
+      <c r="T23" s="52"/>
+      <c r="U23" s="52"/>
+      <c r="V23" s="52"/>
+      <c r="W23" s="52"/>
+      <c r="X23" s="52"/>
+      <c r="Y23" s="52"/>
+      <c r="Z23" s="52"/>
+      <c r="AA23" s="52"/>
+      <c r="AB23" s="52"/>
+      <c r="AC23" s="52"/>
     </row>
     <row r="24" spans="1:29" ht="14.1" customHeight="1">
-      <c r="A24" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
-      <c r="X24" s="54"/>
-      <c r="Y24" s="54"/>
-      <c r="Z24" s="54"/>
-      <c r="AA24" s="54"/>
-      <c r="AB24" s="54"/>
-      <c r="AC24" s="54"/>
+      <c r="A24" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="84"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="X24" s="52"/>
+      <c r="Y24" s="52"/>
+      <c r="Z24" s="52"/>
+      <c r="AA24" s="52"/>
+      <c r="AB24" s="52"/>
+      <c r="AC24" s="52"/>
     </row>
     <row r="25" spans="1:29" ht="6.75" customHeight="1">
-      <c r="A25" s="54"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
@@ -1812,274 +1805,274 @@
     </row>
     <row r="26" spans="1:29" ht="16.5" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="55"/>
+        <v>34</v>
+      </c>
+      <c r="B26" s="53"/>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
-      <c r="X26" s="54"/>
-      <c r="Y26" s="54"/>
-      <c r="Z26" s="54"/>
-      <c r="AA26" s="54"/>
-      <c r="AB26" s="54"/>
-      <c r="AC26" s="54"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
+      <c r="X26" s="52"/>
+      <c r="Y26" s="52"/>
+      <c r="Z26" s="52"/>
+      <c r="AA26" s="52"/>
+      <c r="AB26" s="52"/>
+      <c r="AC26" s="52"/>
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="54"/>
+        <v>9</v>
+      </c>
+      <c r="B27" s="52"/>
     </row>
     <row r="28" spans="1:29" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B28" s="55"/>
+      <c r="B28" s="53"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
-      <c r="X28" s="54"/>
-      <c r="Y28" s="54"/>
-      <c r="Z28" s="54"/>
-      <c r="AA28" s="54"/>
-      <c r="AB28" s="54"/>
-      <c r="AC28" s="54"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="53"/>
+      <c r="X28" s="52"/>
+      <c r="Y28" s="52"/>
+      <c r="Z28" s="52"/>
+      <c r="AA28" s="52"/>
+      <c r="AB28" s="52"/>
+      <c r="AC28" s="52"/>
     </row>
     <row r="29" spans="1:29" ht="17.100000000000001" customHeight="1" thickTop="1">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="32"/>
+      <c r="C29" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="73"/>
+      <c r="E29" s="73"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="74"/>
+    </row>
+    <row r="30" spans="1:29" ht="17.100000000000001" customHeight="1">
+      <c r="A30" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="74" t="s">
+      <c r="B30" s="33"/>
+      <c r="C30" s="75" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="76"/>
+    </row>
+    <row r="31" spans="1:29" ht="17.100000000000001" customHeight="1">
+      <c r="A31" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="33"/>
+      <c r="C31" s="77" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="78"/>
+    </row>
+    <row r="32" spans="1:29" ht="17.100000000000001" customHeight="1">
+      <c r="A32" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="C32" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="79"/>
+      <c r="E32" s="79"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="80"/>
+    </row>
+    <row r="33" spans="1:29" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A33" s="27"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="81"/>
+      <c r="G33" s="82"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="24"/>
+      <c r="T33" s="24"/>
+      <c r="U33" s="24"/>
+      <c r="V33" s="24"/>
+      <c r="W33" s="24"/>
+      <c r="X33" s="24"/>
+      <c r="Y33" s="24"/>
+      <c r="Z33" s="24"/>
+      <c r="AA33" s="24"/>
+      <c r="AB33" s="24"/>
+      <c r="AC33" s="24"/>
+    </row>
+    <row r="34" spans="1:29" ht="17.100000000000001" customHeight="1" thickTop="1">
+      <c r="A34" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="32"/>
+      <c r="C34" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="74"/>
+    </row>
+    <row r="35" spans="1:29" ht="17.100000000000001" customHeight="1">
+      <c r="A35" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="33"/>
+      <c r="C35" s="75" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="75"/>
+      <c r="E35" s="75"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="76"/>
+    </row>
+    <row r="36" spans="1:29" ht="17.100000000000001" customHeight="1">
+      <c r="A36" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="33"/>
+      <c r="C36" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="78"/>
+    </row>
+    <row r="37" spans="1:29" ht="17.100000000000001" customHeight="1">
+      <c r="A37" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="33"/>
+      <c r="C37" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="79"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="80"/>
+    </row>
+    <row r="38" spans="1:29" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A38" s="27"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="81"/>
+      <c r="E38" s="81"/>
+      <c r="F38" s="81"/>
+      <c r="G38" s="82"/>
+    </row>
+    <row r="39" spans="1:29" ht="16.5" thickTop="1">
+      <c r="A39" s="29"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+    </row>
+    <row r="40" spans="1:29" ht="15.75">
+      <c r="A40" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="75"/>
-    </row>
-    <row r="30" spans="1:29" ht="17.100000000000001" customHeight="1">
-      <c r="A30" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="76" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="77"/>
-    </row>
-    <row r="31" spans="1:29" ht="17.100000000000001" customHeight="1">
-      <c r="A31" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="78" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="79"/>
-    </row>
-    <row r="32" spans="1:29" ht="17.100000000000001" customHeight="1">
-      <c r="A32" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="35"/>
-      <c r="C32" s="80" t="s">
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+    </row>
+    <row r="41" spans="1:29" ht="15.75">
+      <c r="A41" s="29"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+    </row>
+    <row r="42" spans="1:29" ht="15.75">
+      <c r="A42" s="29"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+    </row>
+    <row r="43" spans="1:29" ht="15.75">
+      <c r="A43" s="29"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+    </row>
+    <row r="44" spans="1:29" ht="15.75">
+      <c r="A44" s="29"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+    </row>
+    <row r="45" spans="1:29" ht="30" customHeight="1">
+      <c r="A45" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="80"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="81"/>
-    </row>
-    <row r="33" spans="1:29" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A33" s="29"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="82"/>
-      <c r="D33" s="82"/>
-      <c r="E33" s="82"/>
-      <c r="F33" s="82"/>
-      <c r="G33" s="83"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
-      <c r="Q33" s="26"/>
-      <c r="R33" s="26"/>
-      <c r="S33" s="26"/>
-      <c r="T33" s="26"/>
-      <c r="U33" s="26"/>
-      <c r="V33" s="26"/>
-      <c r="W33" s="26"/>
-      <c r="X33" s="26"/>
-      <c r="Y33" s="26"/>
-      <c r="Z33" s="26"/>
-      <c r="AA33" s="26"/>
-      <c r="AB33" s="26"/>
-      <c r="AC33" s="26"/>
-    </row>
-    <row r="34" spans="1:29" ht="17.100000000000001" customHeight="1" thickTop="1">
-      <c r="A34" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="75"/>
-    </row>
-    <row r="35" spans="1:29" ht="17.100000000000001" customHeight="1">
-      <c r="A35" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="76" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="77"/>
-    </row>
-    <row r="36" spans="1:29" ht="17.100000000000001" customHeight="1">
-      <c r="A36" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="78" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="78"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="78"/>
-      <c r="G36" s="79"/>
-    </row>
-    <row r="37" spans="1:29" ht="17.100000000000001" customHeight="1">
-      <c r="A37" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" s="80"/>
-      <c r="E37" s="80"/>
-      <c r="F37" s="80"/>
-      <c r="G37" s="81"/>
-    </row>
-    <row r="38" spans="1:29" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A38" s="29"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="82"/>
-      <c r="G38" s="83"/>
-    </row>
-    <row r="39" spans="1:29" ht="16.5" thickTop="1">
-      <c r="A39" s="31"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35"/>
-    </row>
-    <row r="40" spans="1:29" ht="15.75">
-      <c r="A40" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-    </row>
-    <row r="41" spans="1:29" ht="15.75">
-      <c r="A41" s="31"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35"/>
-    </row>
-    <row r="42" spans="1:29" ht="15.75">
-      <c r="A42" s="31"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-    </row>
-    <row r="43" spans="1:29" ht="15.75">
-      <c r="A43" s="31"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-    </row>
-    <row r="44" spans="1:29" ht="15.75">
-      <c r="A44" s="31"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-    </row>
-    <row r="45" spans="1:29" ht="30" customHeight="1">
-      <c r="A45" s="84" t="s">
+      <c r="B45" s="83"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+    </row>
+    <row r="46" spans="1:29">
+      <c r="A46" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="84"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35"/>
-    </row>
-    <row r="46" spans="1:29">
-      <c r="A46" s="72" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="72"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
+      <c r="B46" s="71"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="25">

</xml_diff>